<commit_message>
Asset Hub TC147 done
</commit_message>
<xml_diff>
--- a/VRT/TestData/AssetNameTestData.xlsx
+++ b/VRT/TestData/AssetNameTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manoj.ghadei\git\VRT\VRT\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81295AED-D4ED-4163-8F1B-EC33E74952B4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97056AAA-8797-4012-A5E7-8CBC8064F8B0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="847" firstSheet="7" activeTab="9" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
+    <workbookView xWindow="0" yWindow="570" windowWidth="20490" windowHeight="10500" tabRatio="847" firstSheet="11" activeTab="18" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
   </bookViews>
   <sheets>
     <sheet name="InvalidAstName" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,8 @@
     <sheet name="InvalidAstLocation" sheetId="16" r:id="rId15"/>
     <sheet name="ValidAstLocation" sheetId="17" r:id="rId16"/>
     <sheet name="AllAssetDetails" sheetId="19" r:id="rId17"/>
-    <sheet name="tc147" sheetId="8" r:id="rId18"/>
+    <sheet name="Sheet1" sheetId="20" r:id="rId18"/>
+    <sheet name="tc147" sheetId="8" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -203,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2014" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2014" uniqueCount="170">
   <si>
     <t>Name</t>
   </si>
@@ -673,24 +674,9 @@
     <t>Asset ID accepts alpha numeric and special characters like space, -,_ ,slash (forward and backward)</t>
   </si>
   <si>
-    <t>147</t>
-  </si>
-  <si>
-    <t>Asset147</t>
-  </si>
-  <si>
-    <t>Manufacturer147</t>
-  </si>
-  <si>
-    <t>Location147</t>
-  </si>
-  <si>
     <t>Model147</t>
   </si>
   <si>
-    <t>Test for successful creation of Asset147 with correct details reflecting in the corresponding Asset tile of Asset Hub page</t>
-  </si>
-  <si>
     <t>Type accepts alpha numeric and special characters like space, -,_ ,slash (forward and backward)</t>
   </si>
   <si>
@@ -710,6 +696,24 @@
   </si>
   <si>
     <t>testAsset</t>
+  </si>
+  <si>
+    <t>Asset147b</t>
+  </si>
+  <si>
+    <t>147b</t>
+  </si>
+  <si>
+    <t>testManufacturer147</t>
+  </si>
+  <si>
+    <t>testLocation147</t>
+  </si>
+  <si>
+    <t>Test for successful creation of Asset147b with correct details reflecting in the corresponding Asset tile of Asset Hub page</t>
+  </si>
+  <si>
+    <t>volume</t>
   </si>
 </sst>
 </file>
@@ -1178,7 +1182,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1204,7 +1208,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -1230,7 +1234,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -1256,7 +1260,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1282,7 +1286,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1308,7 +1312,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1334,7 +1338,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -1360,7 +1364,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -1386,7 +1390,7 @@
         <v>32</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -1412,7 +1416,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -1438,7 +1442,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -1464,7 +1468,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -1490,7 +1494,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -1516,7 +1520,7 @@
         <v>28</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -1542,7 +1546,7 @@
         <v>23</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -1568,7 +1572,7 @@
         <v>24</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -1594,7 +1598,7 @@
         <v>27</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
@@ -1620,7 +1624,7 @@
         <v>29</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -1646,7 +1650,7 @@
         <v>25</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -1672,7 +1676,7 @@
         <v>30</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -1698,7 +1702,7 @@
         <v>31</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -1724,7 +1728,7 @@
         <v>33</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
@@ -1750,7 +1754,7 @@
         <v>34</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
@@ -1776,7 +1780,7 @@
         <v>35</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
@@ -1802,7 +1806,7 @@
         <v>36</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
@@ -1828,7 +1832,7 @@
         <v>37</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
@@ -1859,7 +1863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BF52D8-02BE-4A06-B1E9-330FB0B7B8CA}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
@@ -1900,10 +1904,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1923,10 +1927,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -1946,10 +1950,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -1969,10 +1973,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1992,10 +1996,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2015,10 +2019,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -2038,10 +2042,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -2061,10 +2065,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -2137,10 +2141,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -2163,10 +2167,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -2189,10 +2193,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -2215,10 +2219,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -2241,10 +2245,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2267,10 +2271,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -2293,10 +2297,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -2319,10 +2323,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -2345,10 +2349,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -2371,10 +2375,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -2397,10 +2401,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -2423,10 +2427,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -2449,10 +2453,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -2475,10 +2479,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -2501,10 +2505,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -2527,10 +2531,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -2553,10 +2557,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
@@ -2579,10 +2583,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -2605,10 +2609,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -2631,10 +2635,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -2657,10 +2661,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -2683,10 +2687,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
@@ -2709,10 +2713,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
@@ -2735,10 +2739,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
@@ -2761,10 +2765,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
@@ -2836,10 +2840,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -2859,10 +2863,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -2882,10 +2886,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -2905,10 +2909,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -2928,10 +2932,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2951,10 +2955,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -2974,10 +2978,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -2997,10 +3001,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -3020,10 +3024,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -3043,10 +3047,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -3114,7 +3118,7 @@
         <v>126</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -3126,7 +3130,7 @@
         <v>125</v>
       </c>
       <c r="F2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3134,7 +3138,7 @@
         <v>126</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -3146,7 +3150,7 @@
         <v>125</v>
       </c>
       <c r="F3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3154,7 +3158,7 @@
         <v>126</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -3166,7 +3170,7 @@
         <v>125</v>
       </c>
       <c r="F4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3174,7 +3178,7 @@
         <v>126</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -3186,7 +3190,7 @@
         <v>125</v>
       </c>
       <c r="F5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3194,7 +3198,7 @@
         <v>126</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -3206,7 +3210,7 @@
         <v>125</v>
       </c>
       <c r="F6" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3214,7 +3218,7 @@
         <v>126</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -3226,7 +3230,7 @@
         <v>125</v>
       </c>
       <c r="F7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3234,7 +3238,7 @@
         <v>126</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -3246,7 +3250,7 @@
         <v>125</v>
       </c>
       <c r="F8" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3254,7 +3258,7 @@
         <v>126</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -3266,7 +3270,7 @@
         <v>125</v>
       </c>
       <c r="F9" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3274,7 +3278,7 @@
         <v>126</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -3286,7 +3290,7 @@
         <v>125</v>
       </c>
       <c r="F10" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3294,7 +3298,7 @@
         <v>126</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -3306,7 +3310,7 @@
         <v>125</v>
       </c>
       <c r="F11" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3314,7 +3318,7 @@
         <v>126</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -3326,7 +3330,7 @@
         <v>125</v>
       </c>
       <c r="F12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3334,7 +3338,7 @@
         <v>126</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -3346,7 +3350,7 @@
         <v>125</v>
       </c>
       <c r="F13" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3354,7 +3358,7 @@
         <v>126</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -3366,7 +3370,7 @@
         <v>125</v>
       </c>
       <c r="F14" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -3374,7 +3378,7 @@
         <v>126</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -3386,7 +3390,7 @@
         <v>125</v>
       </c>
       <c r="F15" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -3394,7 +3398,7 @@
         <v>126</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -3406,7 +3410,7 @@
         <v>125</v>
       </c>
       <c r="F16" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -3414,7 +3418,7 @@
         <v>126</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -3426,7 +3430,7 @@
         <v>125</v>
       </c>
       <c r="F17" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -3434,7 +3438,7 @@
         <v>126</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
@@ -3446,7 +3450,7 @@
         <v>125</v>
       </c>
       <c r="F18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -3454,7 +3458,7 @@
         <v>126</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -3466,7 +3470,7 @@
         <v>125</v>
       </c>
       <c r="F19" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -3474,7 +3478,7 @@
         <v>126</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -3486,7 +3490,7 @@
         <v>125</v>
       </c>
       <c r="F20" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -3494,7 +3498,7 @@
         <v>126</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -3506,7 +3510,7 @@
         <v>125</v>
       </c>
       <c r="F21" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -3514,7 +3518,7 @@
         <v>126</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -3526,7 +3530,7 @@
         <v>125</v>
       </c>
       <c r="F22" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -3534,7 +3538,7 @@
         <v>126</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
@@ -3546,7 +3550,7 @@
         <v>125</v>
       </c>
       <c r="F23" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -3554,7 +3558,7 @@
         <v>126</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
@@ -3566,7 +3570,7 @@
         <v>125</v>
       </c>
       <c r="F24" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -3574,7 +3578,7 @@
         <v>126</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
@@ -3586,7 +3590,7 @@
         <v>125</v>
       </c>
       <c r="F25" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3594,7 +3598,7 @@
         <v>126</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>5</v>
@@ -3614,7 +3618,7 @@
         <v>126</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>5</v>
@@ -3675,10 +3679,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -3692,10 +3696,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -3709,10 +3713,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -3726,10 +3730,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -3743,10 +3747,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -3760,10 +3764,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -3777,10 +3781,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -3794,10 +3798,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -3859,7 +3863,7 @@
         <v>133</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -3871,7 +3875,7 @@
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3879,7 +3883,7 @@
         <v>133</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -3891,7 +3895,7 @@
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3899,7 +3903,7 @@
         <v>133</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -3911,7 +3915,7 @@
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3919,7 +3923,7 @@
         <v>133</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -3931,7 +3935,7 @@
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3939,7 +3943,7 @@
         <v>133</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -3951,7 +3955,7 @@
         <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3959,7 +3963,7 @@
         <v>133</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -3971,7 +3975,7 @@
         <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3979,7 +3983,7 @@
         <v>133</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -3991,7 +3995,7 @@
         <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3999,7 +4003,7 @@
         <v>133</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -4011,7 +4015,7 @@
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -4019,7 +4023,7 @@
         <v>133</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -4031,7 +4035,7 @@
         <v>21</v>
       </c>
       <c r="F10" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -4039,7 +4043,7 @@
         <v>133</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -4051,7 +4055,7 @@
         <v>22</v>
       </c>
       <c r="F11" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -4059,7 +4063,7 @@
         <v>133</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -4071,7 +4075,7 @@
         <v>26</v>
       </c>
       <c r="F12" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -4079,7 +4083,7 @@
         <v>133</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -4091,7 +4095,7 @@
         <v>28</v>
       </c>
       <c r="F13" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -4099,7 +4103,7 @@
         <v>133</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -4111,7 +4115,7 @@
         <v>23</v>
       </c>
       <c r="F14" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -4119,7 +4123,7 @@
         <v>133</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -4131,7 +4135,7 @@
         <v>24</v>
       </c>
       <c r="F15" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -4139,7 +4143,7 @@
         <v>133</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -4151,7 +4155,7 @@
         <v>27</v>
       </c>
       <c r="F16" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -4159,7 +4163,7 @@
         <v>133</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -4171,7 +4175,7 @@
         <v>29</v>
       </c>
       <c r="F17" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -4179,7 +4183,7 @@
         <v>133</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
@@ -4191,7 +4195,7 @@
         <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -4199,7 +4203,7 @@
         <v>133</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -4211,7 +4215,7 @@
         <v>30</v>
       </c>
       <c r="F19" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -4219,7 +4223,7 @@
         <v>133</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -4231,7 +4235,7 @@
         <v>31</v>
       </c>
       <c r="F20" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -4239,7 +4243,7 @@
         <v>133</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -4251,7 +4255,7 @@
         <v>33</v>
       </c>
       <c r="F21" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -4259,7 +4263,7 @@
         <v>133</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -4271,7 +4275,7 @@
         <v>34</v>
       </c>
       <c r="F22" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -4279,7 +4283,7 @@
         <v>133</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
@@ -4291,7 +4295,7 @@
         <v>37</v>
       </c>
       <c r="F23" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -4299,7 +4303,7 @@
         <v>133</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
@@ -4311,7 +4315,7 @@
         <v>35</v>
       </c>
       <c r="F24" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -4319,7 +4323,7 @@
         <v>133</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
@@ -4331,7 +4335,7 @@
         <v>36</v>
       </c>
       <c r="F25" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4339,7 +4343,7 @@
         <v>133</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>5</v>
@@ -4359,7 +4363,7 @@
         <v>133</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>5</v>
@@ -4420,10 +4424,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>5</v>
@@ -4437,10 +4441,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>5</v>
@@ -4454,10 +4458,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>5</v>
@@ -4471,10 +4475,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>5</v>
@@ -4488,10 +4492,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>5</v>
@@ -4505,10 +4509,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>5</v>
@@ -4522,10 +4526,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>5</v>
@@ -4539,10 +4543,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>5</v>
@@ -4653,11 +4657,23 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87744AE-AE5A-4295-993D-C7CCE3ABDC2F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26D3E587-13BF-4114-8BD8-3ABD0CCB2044}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4705,28 +4721,28 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>156</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>160</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>152</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>49</v>
@@ -4735,7 +4751,7 @@
         <v>149</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -4782,7 +4798,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -4805,7 +4821,7 @@
         <v>45</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -4828,7 +4844,7 @@
         <v>39</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -4851,7 +4867,7 @@
         <v>40</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -4874,7 +4890,7 @@
         <v>41</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -4897,7 +4913,7 @@
         <v>42</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -4920,7 +4936,7 @@
         <v>43</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -4943,7 +4959,7 @@
         <v>44</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -5015,7 +5031,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>11</v>
@@ -5041,7 +5057,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -5067,7 +5083,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>14</v>
@@ -5093,7 +5109,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>15</v>
@@ -5119,7 +5135,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>16</v>
@@ -5145,7 +5161,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>17</v>
@@ -5171,7 +5187,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>18</v>
@@ -5197,7 +5213,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>19</v>
@@ -5223,7 +5239,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>32</v>
@@ -5249,7 +5265,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>20</v>
@@ -5275,7 +5291,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>21</v>
@@ -5301,7 +5317,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>22</v>
@@ -5327,7 +5343,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>26</v>
@@ -5353,7 +5369,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>28</v>
@@ -5379,7 +5395,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>23</v>
@@ -5405,7 +5421,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>24</v>
@@ -5431,7 +5447,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>27</v>
@@ -5457,7 +5473,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>29</v>
@@ -5483,7 +5499,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>25</v>
@@ -5509,7 +5525,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>30</v>
@@ -5535,7 +5551,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>31</v>
@@ -5561,7 +5577,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>33</v>
@@ -5587,7 +5603,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>34</v>
@@ -5613,7 +5629,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>37</v>
@@ -5639,7 +5655,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>36</v>
@@ -5665,7 +5681,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>35</v>
@@ -5730,7 +5746,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>38</v>
@@ -5753,7 +5769,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>49</v>
@@ -5776,7 +5792,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B4" t="s">
         <v>39</v>
@@ -5799,7 +5815,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B5" t="s">
         <v>40</v>
@@ -5822,7 +5838,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B6" t="s">
         <v>41</v>
@@ -5845,7 +5861,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B7" t="s">
         <v>42</v>
@@ -5868,7 +5884,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B8" t="s">
         <v>43</v>
@@ -5891,7 +5907,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B9" t="s">
         <v>44</v>
@@ -6032,7 +6048,7 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G4" s="3">
         <v>5</v>
@@ -6058,7 +6074,7 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G5" s="3">
         <v>5</v>
@@ -6084,7 +6100,7 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G6" s="3">
         <v>5</v>
@@ -6110,7 +6126,7 @@
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G7" s="3">
         <v>5</v>
@@ -6121,10 +6137,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>18</v>
@@ -6136,7 +6152,7 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G8" s="3">
         <v>5</v>
@@ -6147,10 +6163,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>19</v>
@@ -6162,7 +6178,7 @@
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G9" s="3">
         <v>5</v>
@@ -6173,10 +6189,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>32</v>
@@ -6188,7 +6204,7 @@
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G10" s="3">
         <v>5</v>
@@ -6199,10 +6215,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>20</v>
@@ -6214,7 +6230,7 @@
         <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G11" s="3">
         <v>5</v>
@@ -6225,10 +6241,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>21</v>
@@ -6240,7 +6256,7 @@
         <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G12" s="3">
         <v>5</v>
@@ -6251,10 +6267,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>22</v>
@@ -6266,7 +6282,7 @@
         <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G13" s="3">
         <v>5</v>
@@ -6277,10 +6293,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>26</v>
@@ -6292,7 +6308,7 @@
         <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G14" s="3">
         <v>5</v>
@@ -6303,10 +6319,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>28</v>
@@ -6318,7 +6334,7 @@
         <v>7</v>
       </c>
       <c r="F15" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G15" s="3">
         <v>5</v>
@@ -6329,10 +6345,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>23</v>
@@ -6344,7 +6360,7 @@
         <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G16" s="3">
         <v>5</v>
@@ -6355,10 +6371,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>24</v>
@@ -6370,7 +6386,7 @@
         <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G17" s="3">
         <v>5</v>
@@ -6381,10 +6397,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>27</v>
@@ -6396,7 +6412,7 @@
         <v>7</v>
       </c>
       <c r="F18" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G18" s="3">
         <v>5</v>
@@ -6407,10 +6423,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>29</v>
@@ -6422,7 +6438,7 @@
         <v>7</v>
       </c>
       <c r="F19" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G19" s="3">
         <v>5</v>
@@ -6433,10 +6449,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>25</v>
@@ -6448,7 +6464,7 @@
         <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G20" s="3">
         <v>5</v>
@@ -6459,10 +6475,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>30</v>
@@ -6474,7 +6490,7 @@
         <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G21" s="3">
         <v>5</v>
@@ -6485,10 +6501,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>31</v>
@@ -6500,7 +6516,7 @@
         <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G22" s="3">
         <v>5</v>
@@ -6511,10 +6527,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>33</v>
@@ -6526,7 +6542,7 @@
         <v>7</v>
       </c>
       <c r="F23" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G23" s="3">
         <v>5</v>
@@ -6537,10 +6553,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>34</v>
@@ -6552,7 +6568,7 @@
         <v>7</v>
       </c>
       <c r="F24" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G24" s="3">
         <v>5</v>
@@ -6563,10 +6579,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>37</v>
@@ -6578,7 +6594,7 @@
         <v>7</v>
       </c>
       <c r="F25" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G25" s="3">
         <v>5</v>
@@ -6589,10 +6605,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>36</v>
@@ -6604,7 +6620,7 @@
         <v>7</v>
       </c>
       <c r="F26" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G26" s="3">
         <v>5</v>
@@ -6615,10 +6631,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>35</v>
@@ -6630,7 +6646,7 @@
         <v>7</v>
       </c>
       <c r="F27" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G27" s="3">
         <v>5</v>
@@ -6683,10 +6699,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>38</v>
@@ -6706,10 +6722,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>49</v>
@@ -6729,10 +6745,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C4" t="s">
         <v>39</v>
@@ -6752,10 +6768,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C5" t="s">
         <v>40</v>
@@ -6775,10 +6791,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C6" t="s">
         <v>41</v>
@@ -6798,10 +6814,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C7" t="s">
         <v>42</v>
@@ -6821,10 +6837,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C8" t="s">
         <v>43</v>
@@ -6844,10 +6860,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C9" t="s">
         <v>44</v>
@@ -7191,10 +7207,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -7214,10 +7230,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -7237,10 +7253,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -7260,10 +7276,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -7283,10 +7299,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
@@ -7306,10 +7322,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -7329,10 +7345,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -7352,10 +7368,10 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -7375,10 +7391,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -7398,10 +7414,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
@@ -7421,10 +7437,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
@@ -7444,10 +7460,10 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
@@ -7503,10 +7519,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>58</v>
@@ -7523,10 +7539,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>58</v>
@@ -7543,10 +7559,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>58</v>
@@ -7563,10 +7579,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>58</v>
@@ -7583,10 +7599,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>58</v>
@@ -7603,10 +7619,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>58</v>
@@ -7623,10 +7639,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>58</v>
@@ -7643,10 +7659,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>58</v>
@@ -8209,10 +8225,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -8235,10 +8251,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -8261,10 +8277,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
@@ -8287,10 +8303,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
@@ -8313,10 +8329,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
@@ -8339,10 +8355,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
@@ -8365,10 +8381,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
@@ -8391,10 +8407,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C28" t="s">
         <v>5</v>
@@ -8417,10 +8433,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
@@ -8443,10 +8459,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C30" t="s">
         <v>5</v>
@@ -8469,10 +8485,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C31" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Asset Hub Page Test cases added for ASST001,ASST002,ASST004, ASST005,ASST006 & ASST007
</commit_message>
<xml_diff>
--- a/VRT/TestData/AssetNameTestData.xlsx
+++ b/VRT/TestData/AssetNameTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manoj.ghadei\git\VRT\VRT\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97056AAA-8797-4012-A5E7-8CBC8064F8B0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01FB6534-9C31-4C74-8562-9CD69A7776B7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="570" windowWidth="20490" windowHeight="10500" tabRatio="847" firstSheet="11" activeTab="18" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="847" firstSheet="11" activeTab="19" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
   </bookViews>
   <sheets>
     <sheet name="InvalidAstName" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,7 @@
     <sheet name="AllAssetDetails" sheetId="19" r:id="rId17"/>
     <sheet name="Sheet1" sheetId="20" r:id="rId18"/>
     <sheet name="tc147" sheetId="8" r:id="rId19"/>
+    <sheet name="tc149" sheetId="21" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -203,8 +204,110 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ghadei, Manoj (Amphenol-AS)</author>
+  </authors>
+  <commentList>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{EC7488E6-A897-4FD3-BAB5-85E9EF760D77}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ghadei, Manoj (Amphenol-AS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert Only +ve Integer Data</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{48F36AC3-FA47-41A9-AC2F-ADF178E66A37}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ghadei, Manoj (Amphenol-AS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert Default Size Units Like cu ft/m/in</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{0F9BD116-B952-4ACD-A2CD-8F199466C54E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ghadei, Manoj (Amphenol-AS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert Only +ve Integer Data between 1-24
+- And </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DO NOT</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> enter same value as entered in Size field</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2014" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2036" uniqueCount="177">
   <si>
     <t>Name</t>
   </si>
@@ -714,13 +817,34 @@
   </si>
   <si>
     <t>volume</t>
+  </si>
+  <si>
+    <t>Asset149</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>149-Manufacturer</t>
+  </si>
+  <si>
+    <t>149location</t>
+  </si>
+  <si>
+    <t>Model149</t>
+  </si>
+  <si>
+    <t>cu ft</t>
+  </si>
+  <si>
+    <t>Test for successful creation of Asset149 with correct details reflecting in the corresponding Asset tile of Asset Hub page</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -748,6 +872,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -835,6 +972,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Ghadei, Manoj (Amphenol-AS)" id="{2B5AC18C-CBD4-4A93-B399-6D04820C6454}" userId="Ghadei, Manoj (Amphenol-AS)" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4672,7 +4815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26D3E587-13BF-4114-8BD8-3ABD0CCB2044}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -4980,6 +5123,98 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2977AC3-E2DD-4754-BCA4-066831CE45B8}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Latest Update, ASST014 TC added under Asset Hub page
</commit_message>
<xml_diff>
--- a/VRT/TestData/AssetNameTestData.xlsx
+++ b/VRT/TestData/AssetNameTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manoj.ghadei\git\VRT\VRT\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01FB6534-9C31-4C74-8562-9CD69A7776B7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0723D690-2EE4-4EBF-9A3F-23F2600374EC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="847" firstSheet="11" activeTab="19" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="847" firstSheet="12" activeTab="21" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
   </bookViews>
   <sheets>
     <sheet name="InvalidAstName" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,8 @@
     <sheet name="Sheet1" sheetId="20" r:id="rId18"/>
     <sheet name="tc147" sheetId="8" r:id="rId19"/>
     <sheet name="tc149" sheetId="21" r:id="rId20"/>
+    <sheet name="tcasst011" sheetId="22" r:id="rId21"/>
+    <sheet name="tcasst014" sheetId="23" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -306,8 +308,308 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ghadei, Manoj (Amphenol-AS)</author>
+  </authors>
+  <commentList>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{4CF7F98A-9EDA-400C-AF1A-312A4DD9E354}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ghadei, Manoj (Amphenol-AS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert Only +ve Integer Data</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{D8EA7BD9-0F3F-44D6-9A56-B87CB1CE311D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ghadei, Manoj (Amphenol-AS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert Default Size Units Like cu ft/m/in</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{9886B2F3-C1AD-40A7-A0D3-EAF19B360FFC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ghadei, Manoj (Amphenol-AS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert Only +ve Integer Data between 1-24
+- And </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DO NOT</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> enter same value as entered in Size field</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ghadei, Manoj (Amphenol-AS)</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{637C303C-5010-42AF-A522-AC76EAC6092D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ghadei, Manoj (Amphenol-AS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert Unique data</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{F4CCC0A0-87E6-4986-8182-0D45D7E57D71}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ghadei, Manoj (Amphenol-AS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert Unique data</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{C26356A2-85F8-49E1-BF71-D3E706EF10C8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ghadei, Manoj (Amphenol-AS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert data with the 1st letter as Unique</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{C15F0743-5C8F-4C39-906F-078889D33126}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ghadei, Manoj (Amphenol-AS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert data with the 1st letter as Unique</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{0DEADBE6-39AD-40FD-9319-9F5DF77521A0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ghadei, Manoj (Amphenol-AS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert Only +ve Integer Data</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{4394BABF-E99F-4DC2-B801-4E4B33AFBF14}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ghadei, Manoj (Amphenol-AS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert Default Size Units Like cu ft/m/in</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{9F7EDF02-5713-4215-9C51-10A935007AC2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ghadei, Manoj (Amphenol-AS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert Only +ve Integer Data between 1-24
+- And </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DO NOT</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> enter same value as entered in Size field</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2036" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2080" uniqueCount="188">
   <si>
     <t>Name</t>
   </si>
@@ -838,6 +1140,39 @@
   </si>
   <si>
     <t>Test for successful creation of Asset149 with correct details reflecting in the corresponding Asset tile of Asset Hub page</t>
+  </si>
+  <si>
+    <t>Asset011</t>
+  </si>
+  <si>
+    <t>Model-11</t>
+  </si>
+  <si>
+    <t>ASST011-Verify if click on the Type filter user is able to filter all the assets correctly by Asset Type</t>
+  </si>
+  <si>
+    <t>Model-14</t>
+  </si>
+  <si>
+    <t>1-Manufacturer</t>
+  </si>
+  <si>
+    <t>1-location</t>
+  </si>
+  <si>
+    <t>Asset019</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>6-Manufacturer</t>
+  </si>
+  <si>
+    <t>6-location</t>
+  </si>
+  <si>
+    <t>ASST014-</t>
   </si>
 </sst>
 </file>
@@ -5130,7 +5465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2977AC3-E2DD-4754-BCA4-066831CE45B8}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -5210,6 +5545,190 @@
       </c>
       <c r="K2" s="12" t="s">
         <v>176</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0EC7E7-0A30-41F4-9875-DC335ECFE7AE}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36C667C-6956-48CC-B8BF-D3D1D233432F}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ASST015 TC updated for Asset Hub page & Allure reporting disbaled
</commit_message>
<xml_diff>
--- a/VRT/TestData/AssetNameTestData.xlsx
+++ b/VRT/TestData/AssetNameTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manoj.ghadei\git\VRT\VRT\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0723D690-2EE4-4EBF-9A3F-23F2600374EC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AA6BC0-7198-422A-BAA7-0CA0431A2DFB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="847" firstSheet="12" activeTab="21" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="20490" windowHeight="10500" tabRatio="847" firstSheet="12" activeTab="21" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
   </bookViews>
   <sheets>
     <sheet name="InvalidAstName" sheetId="1" r:id="rId1"/>
@@ -609,7 +609,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2080" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2124" uniqueCount="199">
   <si>
     <t>Name</t>
   </si>
@@ -1142,15 +1142,9 @@
     <t>Test for successful creation of Asset149 with correct details reflecting in the corresponding Asset tile of Asset Hub page</t>
   </si>
   <si>
-    <t>Asset011</t>
-  </si>
-  <si>
     <t>Model-11</t>
   </si>
   <si>
-    <t>ASST011-Verify if click on the Type filter user is able to filter all the assets correctly by Asset Type</t>
-  </si>
-  <si>
     <t>Model-14</t>
   </si>
   <si>
@@ -1160,19 +1154,58 @@
     <t>1-location</t>
   </si>
   <si>
-    <t>Asset019</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>6-Manufacturer</t>
-  </si>
-  <si>
-    <t>6-location</t>
-  </si>
-  <si>
-    <t>ASST014-</t>
+    <t>Asset01</t>
+  </si>
+  <si>
+    <t>ASST014- Test</t>
+  </si>
+  <si>
+    <t>Asset02</t>
+  </si>
+  <si>
+    <t>Model-15</t>
+  </si>
+  <si>
+    <t>Asset03</t>
+  </si>
+  <si>
+    <t>Model-16</t>
+  </si>
+  <si>
+    <t>2-Manufacturer</t>
+  </si>
+  <si>
+    <t>ASST011-Test</t>
+  </si>
+  <si>
+    <t>Model-12</t>
+  </si>
+  <si>
+    <t>Model-13</t>
+  </si>
+  <si>
+    <t>Sterilizer</t>
+  </si>
+  <si>
+    <t>3-Manufacturer</t>
+  </si>
+  <si>
+    <t>2-location</t>
+  </si>
+  <si>
+    <t>3-location</t>
+  </si>
+  <si>
+    <t>1-Man</t>
+  </si>
+  <si>
+    <t>1-Manuf</t>
+  </si>
+  <si>
+    <t>1-locate</t>
+  </si>
+  <si>
+    <t>1-locatio</t>
   </si>
 </sst>
 </file>
@@ -5466,7 +5499,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5555,10 +5588,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0EC7E7-0A30-41F4-9875-DC335ECFE7AE}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5576,7 +5609,7 @@
       <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
@@ -5606,22 +5639,22 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>177</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>178</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>152</v>
@@ -5636,7 +5669,77 @@
         <v>149</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>179</v>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -5647,10 +5750,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36C667C-6956-48CC-B8BF-D3D1D233432F}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5671,7 +5774,7 @@
       <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="10" t="s">
@@ -5698,22 +5801,22 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>184</v>
+        <v>48</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>152</v>
@@ -5728,7 +5831,77 @@
         <v>149</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>187</v>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
VRT project Updated as on 13 Nov
</commit_message>
<xml_diff>
--- a/VRT/TestData/AssetNameTestData.xlsx
+++ b/VRT/TestData/AssetNameTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manoj.ghadei\git\VRT\VRT\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F3E85F-002A-44AA-82F9-DC2FDBBDC686}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065ABF8D-78C1-47CB-943A-43BAEDE2DC67}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="847" firstSheet="19" activeTab="26" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="847" firstSheet="19" activeTab="27" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
   </bookViews>
   <sheets>
     <sheet name="ASST02" sheetId="2" r:id="rId1"/>
@@ -40,12 +40,13 @@
     <sheet name="ASST41" sheetId="34" r:id="rId25"/>
     <sheet name="ASST42" sheetId="36" r:id="rId26"/>
     <sheet name="AssetAllData" sheetId="19" r:id="rId27"/>
-    <sheet name="tcasst011" sheetId="22" r:id="rId28"/>
-    <sheet name="tc147" sheetId="8" r:id="rId29"/>
-    <sheet name="tc149" sheetId="21" r:id="rId30"/>
-    <sheet name="tcasst014" sheetId="23" r:id="rId31"/>
-    <sheet name="Sheet1" sheetId="26" r:id="rId32"/>
-    <sheet name="Sheet3" sheetId="35" r:id="rId33"/>
+    <sheet name="ASST49" sheetId="37" r:id="rId28"/>
+    <sheet name="tcasst011" sheetId="22" r:id="rId29"/>
+    <sheet name="tc147" sheetId="8" r:id="rId30"/>
+    <sheet name="tc149" sheetId="21" r:id="rId31"/>
+    <sheet name="tcasst014" sheetId="23" r:id="rId32"/>
+    <sheet name="Sheet1" sheetId="26" r:id="rId33"/>
+    <sheet name="Sheet3" sheetId="35" r:id="rId34"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -374,7 +375,7 @@
     <author>Ghadei, Manoj (Amphenol-AS)</author>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{4CF7F98A-9EDA-400C-AF1A-312A4DD9E354}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{4AED6921-04CB-439E-B61F-45D21FECB987}">
       <text>
         <r>
           <rPr>
@@ -398,7 +399,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{D8EA7BD9-0F3F-44D6-9A56-B87CB1CE311D}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{9108BBC9-51AC-411B-9B3E-6623C8E3D918}">
       <text>
         <r>
           <rPr>
@@ -418,11 +419,12 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Insert Default Size Units Like cu ft/m/in</t>
+- Enter todays date
+-Insert Date in mm-dd-YYYY format</t>
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{9886B2F3-C1AD-40A7-A0D3-EAF19B360FFC}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{4852396F-8461-4CDE-BA96-0FF3DA5E2F35}">
       <text>
         <r>
           <rPr>
@@ -476,7 +478,7 @@
     <author>Ghadei, Manoj (Amphenol-AS)</author>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{4C2154AD-42EF-4B40-B614-C0E650AE12A9}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{4CF7F98A-9EDA-400C-AF1A-312A4DD9E354}">
       <text>
         <r>
           <rPr>
@@ -500,7 +502,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{A1D49A09-E5F3-41F2-8E60-B0135B0BA616}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{D8EA7BD9-0F3F-44D6-9A56-B87CB1CE311D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ghadei, Manoj (Amphenol-AS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert Default Size Units Like cu ft/m/in</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{9886B2F3-C1AD-40A7-A0D3-EAF19B360FFC}">
       <text>
         <r>
           <rPr>
@@ -554,7 +580,7 @@
     <author>Ghadei, Manoj (Amphenol-AS)</author>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{EC7488E6-A897-4FD3-BAB5-85E9EF760D77}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{4C2154AD-42EF-4B40-B614-C0E650AE12A9}">
       <text>
         <r>
           <rPr>
@@ -578,31 +604,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{48F36AC3-FA47-41A9-AC2F-ADF178E66A37}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Ghadei, Manoj (Amphenol-AS):</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Insert Default Size Units Like cu ft/m/in</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{0F9BD116-B952-4ACD-A2CD-8F199466C54E}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{A1D49A09-E5F3-41F2-8E60-B0135B0BA616}">
       <text>
         <r>
           <rPr>
@@ -651,6 +653,108 @@
 </file>
 
 <file path=xl/comments15.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ghadei, Manoj (Amphenol-AS)</author>
+  </authors>
+  <commentList>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{EC7488E6-A897-4FD3-BAB5-85E9EF760D77}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ghadei, Manoj (Amphenol-AS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert Only +ve Integer Data</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{48F36AC3-FA47-41A9-AC2F-ADF178E66A37}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ghadei, Manoj (Amphenol-AS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert Default Size Units Like cu ft/m/in</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{0F9BD116-B952-4ACD-A2CD-8F199466C54E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ghadei, Manoj (Amphenol-AS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert Only +ve Integer Data between 1-24
+- And </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DO NOT</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> enter same value as entered in Size field</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments16.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ghadei, Manoj (Amphenol-AS)</author>
@@ -1665,7 +1769,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2366" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2390" uniqueCount="241">
   <si>
     <t>Name</t>
   </si>
@@ -2376,6 +2480,18 @@
   </si>
   <si>
     <t>ASSTNew</t>
+  </si>
+  <si>
+    <t>ASST49</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>Test Description for ASST49</t>
+  </si>
+  <si>
+    <t>11-13-2019</t>
   </si>
 </sst>
 </file>
@@ -8176,7 +8292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B6BA4E0-0C67-45A7-85A8-9BF5353A1E8A}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -8272,6 +8388,105 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E963294-A9BA-4C6F-8828-8A0493CE8586}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>239</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0EC7E7-0A30-41F4-9875-DC335ECFE7AE}">
   <dimension ref="A1:K4"/>
   <sheetViews>
@@ -8425,98 +8640,6 @@
       </c>
       <c r="K4" s="12" t="s">
         <v>176</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26D3E587-13BF-4114-8BD8-3ABD0CCB2044}">
-  <dimension ref="A1:K2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -8748,6 +8871,98 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26D3E587-13BF-4114-8BD8-3ABD0CCB2044}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2977AC3-E2DD-4754-BCA4-066831CE45B8}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -8839,7 +9054,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36C667C-6956-48CC-B8BF-D3D1D233432F}">
   <dimension ref="A1:K4"/>
   <sheetViews>
@@ -9001,7 +9216,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E86BD1EC-71B3-42BE-BB2A-D697838FB4B1}">
   <dimension ref="K1"/>
   <sheetViews>
@@ -9014,7 +9229,7 @@
     <row r="1" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K1" s="4" t="str">
         <f ca="1">TEXT(TODAY(),"mm-dd-YYYY")</f>
-        <v>11-12-2019</v>
+        <v>11-14-2019</v>
       </c>
     </row>
   </sheetData>
@@ -9022,7 +9237,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D3E2A5-C485-4106-9941-FABDA2FA890E}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
VRT Updated for Asset Creation Page class for Date change format from 11-18-2019 to 11/18/2019
</commit_message>
<xml_diff>
--- a/VRT/TestData/AssetNameTestData.xlsx
+++ b/VRT/TestData/AssetNameTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manoj.ghadei\git\VRT\VRT\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA9B923-BC4E-40C7-A89E-84E3554808FF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525988D6-27ED-4905-8400-909B0B63C53A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="847" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="847" firstSheet="15" activeTab="15" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
   </bookViews>
   <sheets>
     <sheet name="ASST02" sheetId="2" r:id="rId1"/>
@@ -107,7 +107,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Insert Date in mm-dd-yyyy format</t>
+Insert Date in mm/dd/YYYY format</t>
         </r>
       </text>
     </comment>
@@ -209,7 +209,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Insert Date in mm-dd-yyyy format</t>
+Insert Date in mm/dd/YYYY format</t>
         </r>
       </text>
     </comment>
@@ -311,7 +311,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Insert Date in mm-dd-yyyy format</t>
+Insert Date in mm/dd/YYYY</t>
         </r>
       </text>
     </comment>
@@ -414,7 +414,7 @@
           </rPr>
           <t xml:space="preserve">
 - Enter todays date
--Insert Date in mm-dd-YYYY format</t>
+-Insert Date in mm/dd/YYYY format</t>
         </r>
       </text>
     </comment>
@@ -516,7 +516,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Insert Date in mm-dd-yyyy format</t>
+Insert Date in mm/dd/YYYY format</t>
         </r>
       </text>
     </comment>
@@ -618,7 +618,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Insert Date in mm-dd-yyyy format</t>
+Insert Date in mm/dd/YYYY format</t>
         </r>
       </text>
     </comment>
@@ -720,7 +720,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Insert Date in mm-dd-yyyy format</t>
+Insert Date in mm/dd/YYYY format</t>
         </r>
       </text>
     </comment>
@@ -822,7 +822,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Insert Date in mm-dd-yyyy format</t>
+Insert Date in mm/dd/YYYY format</t>
         </r>
       </text>
     </comment>
@@ -924,7 +924,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Insert Date in mm-dd-yyyy format</t>
+Insert Date in mm/dd/YYYY format</t>
         </r>
       </text>
     </comment>
@@ -1026,7 +1026,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Insert Date in mm-dd-yyyy format</t>
+Insert Date in mm/dd/YYYY format</t>
         </r>
       </text>
     </comment>
@@ -1128,7 +1128,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Insert Date in mm-dd-yyyy format</t>
+Insert Date in mm/dd/YYYYy format</t>
         </r>
       </text>
     </comment>
@@ -1230,7 +1230,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Insert Date in mm-dd-yyyy format</t>
+Insert Date in mm/dd/YYYY format</t>
         </r>
       </text>
     </comment>
@@ -1283,7 +1283,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2258" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2258" uniqueCount="202">
   <si>
     <t>Name</t>
   </si>
@@ -1765,9 +1765,6 @@
     <t>Validation Date</t>
   </si>
   <si>
-    <t>11-08-2019</t>
-  </si>
-  <si>
     <t>Bath</t>
   </si>
   <si>
@@ -1798,15 +1795,9 @@
     <t>Test Description for ASST32c</t>
   </si>
   <si>
-    <t>10-09-2019</t>
-  </si>
-  <si>
     <t>Test Description for ASST32b</t>
   </si>
   <si>
-    <t>11-09-2019</t>
-  </si>
-  <si>
     <t>ASST35</t>
   </si>
   <si>
@@ -1849,9 +1840,6 @@
     <t>39</t>
   </si>
   <si>
-    <t>11-11-2019</t>
-  </si>
-  <si>
     <t>Test Description for ASST39</t>
   </si>
   <si>
@@ -1861,9 +1849,6 @@
     <t>41</t>
   </si>
   <si>
-    <t>11-12-2019</t>
-  </si>
-  <si>
     <t>Test Description for ASST41</t>
   </si>
   <si>
@@ -1894,7 +1879,16 @@
     <t>Test Description for ASST49</t>
   </si>
   <si>
-    <t>11-13-2019</t>
+    <t>11/11/2019</t>
+  </si>
+  <si>
+    <t>11/09/2019</t>
+  </si>
+  <si>
+    <t>11/08/2019</t>
+  </si>
+  <si>
+    <t>10/09/2019</t>
   </si>
 </sst>
 </file>
@@ -2335,7 +2329,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AAF0D48-3FFE-4E63-90D8-6D4600BE85B6}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -5267,7 +5261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89930B9C-F1A9-4890-AFB9-2EA6D8CB06AA}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
     </sheetView>
@@ -5971,7 +5965,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6022,13 +6016,13 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>164</v>
-      </c>
       <c r="C2" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>6</v>
@@ -6046,7 +6040,7 @@
         <v>157</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="J2" s="12" t="s">
         <v>48</v>
@@ -6055,7 +6049,7 @@
         <v>158</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -6070,7 +6064,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6121,13 +6115,13 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>166</v>
-      </c>
       <c r="C2" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>6</v>
@@ -6145,16 +6139,16 @@
         <v>157</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="J2" s="12" t="s">
         <v>48</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -6169,7 +6163,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6220,13 +6214,13 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>169</v>
-      </c>
       <c r="C2" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>6</v>
@@ -6244,7 +6238,7 @@
         <v>157</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>173</v>
+        <v>199</v>
       </c>
       <c r="J2" s="12" t="s">
         <v>48</v>
@@ -6253,7 +6247,7 @@
         <v>142</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -6995,7 +6989,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7046,10 +7040,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>5</v>
@@ -7070,7 +7064,7 @@
         <v>157</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>173</v>
+        <v>199</v>
       </c>
       <c r="J2" s="12" t="s">
         <v>48</v>
@@ -7079,7 +7073,7 @@
         <v>158</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -7094,7 +7088,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7145,10 +7139,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>5</v>
@@ -7169,7 +7163,7 @@
         <v>157</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>173</v>
+        <v>199</v>
       </c>
       <c r="J2" s="12" t="s">
         <v>48</v>
@@ -7178,7 +7172,7 @@
         <v>158</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -7193,7 +7187,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7244,10 +7238,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>5</v>
@@ -7268,7 +7262,7 @@
         <v>157</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>173</v>
+        <v>199</v>
       </c>
       <c r="J2" s="12" t="s">
         <v>48</v>
@@ -7277,7 +7271,7 @@
         <v>158</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -7292,7 +7286,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7343,10 +7337,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>5</v>
@@ -7367,7 +7361,7 @@
         <v>157</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>173</v>
+        <v>199</v>
       </c>
       <c r="J2" s="12" t="s">
         <v>48</v>
@@ -7376,7 +7370,7 @@
         <v>158</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -7391,7 +7385,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7442,10 +7436,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>5</v>
@@ -7466,7 +7460,7 @@
         <v>157</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="J2" s="12" t="s">
         <v>48</v>
@@ -7475,7 +7469,7 @@
         <v>158</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -7490,7 +7484,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7541,10 +7535,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>5</v>
@@ -7565,7 +7559,7 @@
         <v>157</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="J2" s="12" t="s">
         <v>48</v>
@@ -7574,7 +7568,7 @@
         <v>158</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -7589,7 +7583,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:L2"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7640,10 +7634,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>5</v>
@@ -7664,7 +7658,7 @@
         <v>157</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="J2" s="12" t="s">
         <v>48</v>
@@ -7673,7 +7667,7 @@
         <v>158</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -7688,7 +7682,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7739,10 +7733,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>5</v>
@@ -7763,7 +7757,7 @@
         <v>157</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="J2" s="12" t="s">
         <v>48</v>
@@ -7772,7 +7766,7 @@
         <v>158</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -7787,7 +7781,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7838,10 +7832,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>5</v>
@@ -7862,7 +7856,7 @@
         <v>157</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="J2" s="12" t="s">
         <v>48</v>
@@ -7871,7 +7865,7 @@
         <v>158</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ASST 32a TC updated
</commit_message>
<xml_diff>
--- a/VRT/TestData/AssetNameTestData.xlsx
+++ b/VRT/TestData/AssetNameTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manoj.ghadei\git\VRT\VRT\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525988D6-27ED-4905-8400-909B0B63C53A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430FD40B-C60A-4A1F-8F45-8AE8C8FDF833}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="847" firstSheet="15" activeTab="15" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
+    <workbookView xWindow="0" yWindow="510" windowWidth="20490" windowHeight="10560" tabRatio="847" firstSheet="15" activeTab="17" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
   </bookViews>
   <sheets>
     <sheet name="ASST02" sheetId="2" r:id="rId1"/>
@@ -29,18 +29,19 @@
     <sheet name="ASST25" sheetId="10" r:id="rId14"/>
     <sheet name="ASST28" sheetId="13" r:id="rId15"/>
     <sheet name="ASST29" sheetId="12" r:id="rId16"/>
-    <sheet name="ASST32a" sheetId="25" r:id="rId17"/>
-    <sheet name="ASST32b" sheetId="27" r:id="rId18"/>
-    <sheet name="ASST32c" sheetId="28" r:id="rId19"/>
-    <sheet name="ASST35" sheetId="29" r:id="rId20"/>
-    <sheet name="ASST36" sheetId="30" r:id="rId21"/>
-    <sheet name="ASST37" sheetId="31" r:id="rId22"/>
-    <sheet name="ASST38" sheetId="32" r:id="rId23"/>
-    <sheet name="ASST39" sheetId="33" r:id="rId24"/>
-    <sheet name="ASST41" sheetId="34" r:id="rId25"/>
-    <sheet name="ASST42" sheetId="36" r:id="rId26"/>
-    <sheet name="AssetAllData" sheetId="19" r:id="rId27"/>
-    <sheet name="ASST49" sheetId="37" r:id="rId28"/>
+    <sheet name="ASST30b" sheetId="38" r:id="rId17"/>
+    <sheet name="ASST32a" sheetId="25" r:id="rId18"/>
+    <sheet name="ASST32b" sheetId="27" r:id="rId19"/>
+    <sheet name="ASST32c" sheetId="28" r:id="rId20"/>
+    <sheet name="ASST35" sheetId="29" r:id="rId21"/>
+    <sheet name="ASST36" sheetId="30" r:id="rId22"/>
+    <sheet name="ASST37" sheetId="31" r:id="rId23"/>
+    <sheet name="ASST38" sheetId="32" r:id="rId24"/>
+    <sheet name="ASST39" sheetId="33" r:id="rId25"/>
+    <sheet name="ASST41" sheetId="34" r:id="rId26"/>
+    <sheet name="ASST42" sheetId="36" r:id="rId27"/>
+    <sheet name="AssetAllData" sheetId="19" r:id="rId28"/>
+    <sheet name="ASST49" sheetId="37" r:id="rId29"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -63,7 +64,41 @@
     <author>Ghadei, Manoj (Amphenol-AS)</author>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{84346A25-2952-4B5F-9579-5E730E106FC8}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{C650163B-C4A9-4AAC-83BD-CE5E28C8E449}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ghadei, Manoj (Amphenol-AS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Enter the expected Last Validated Date to be set for a new Asset in mm/dd/yyyy format</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ghadei, Manoj (Amphenol-AS)</author>
+  </authors>
+  <commentList>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{B9C7326C-C882-4F9F-B294-800778C100BD}">
       <text>
         <r>
           <rPr>
@@ -87,7 +122,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{449D7C87-121A-4A11-8277-E2F0545BDC34}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{6500FF9D-5C4E-4EC5-A4F8-D633C1F80FD2}">
       <text>
         <r>
           <rPr>
@@ -111,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{C53B6AAB-3A36-42F2-9EF2-BCDF8321365F}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{E9455E97-BB05-4C05-A7FE-74EB4C5EB3B0}">
       <text>
         <r>
           <rPr>
@@ -159,7 +194,7 @@
 </comments>
 </file>
 
-<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ghadei, Manoj (Amphenol-AS)</author>
@@ -261,7 +296,7 @@
 </comments>
 </file>
 
-<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ghadei, Manoj (Amphenol-AS)</author>
@@ -363,7 +398,7 @@
 </comments>
 </file>
 
-<file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments13.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ghadei, Manoj (Amphenol-AS)</author>
@@ -472,6 +507,108 @@
     <author>Ghadei, Manoj (Amphenol-AS)</author>
   </authors>
   <commentList>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{84346A25-2952-4B5F-9579-5E730E106FC8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ghadei, Manoj (Amphenol-AS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert Only +ve Integer Data</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{449D7C87-121A-4A11-8277-E2F0545BDC34}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ghadei, Manoj (Amphenol-AS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert Todays Date in mm/dd/YYYY format</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{C53B6AAB-3A36-42F2-9EF2-BCDF8321365F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ghadei, Manoj (Amphenol-AS):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert Only +ve Integer Data between 1-24
+- And </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DO NOT</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> enter same value as entered in Size field</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ghadei, Manoj (Amphenol-AS)</author>
+  </authors>
+  <commentList>
     <comment ref="G1" authorId="0" shapeId="0" xr:uid="{DD8C3CF4-F1D4-450E-B15A-C0B631B69535}">
       <text>
         <r>
@@ -516,7 +653,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Insert Date in mm/dd/YYYY format</t>
+Insert Todays Date in mm/dd/YYYY format</t>
         </r>
       </text>
     </comment>
@@ -568,7 +705,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ghadei, Manoj (Amphenol-AS)</author>
@@ -670,7 +807,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ghadei, Manoj (Amphenol-AS)</author>
@@ -772,7 +909,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ghadei, Manoj (Amphenol-AS)</author>
@@ -874,7 +1011,7 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ghadei, Manoj (Amphenol-AS)</author>
@@ -976,7 +1113,7 @@
 </comments>
 </file>
 
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ghadei, Manoj (Amphenol-AS)</author>
@@ -1078,7 +1215,7 @@
 </comments>
 </file>
 
-<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ghadei, Manoj (Amphenol-AS)</author>
@@ -1180,110 +1317,8 @@
 </comments>
 </file>
 
-<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Ghadei, Manoj (Amphenol-AS)</author>
-  </authors>
-  <commentList>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{B9C7326C-C882-4F9F-B294-800778C100BD}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ghadei, Manoj (Amphenol-AS):</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Insert Only +ve Integer Data</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{6500FF9D-5C4E-4EC5-A4F8-D633C1F80FD2}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Ghadei, Manoj (Amphenol-AS):</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Insert Date in mm/dd/YYYY format</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{E9455E97-BB05-4C05-A7FE-74EB4C5EB3B0}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ghadei, Manoj (Amphenol-AS):</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Insert Only +ve Integer Data between 1-24
-- And </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>DO NOT</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> enter same value as entered in Size field</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2258" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2260" uniqueCount="203">
   <si>
     <t>Name</t>
   </si>
@@ -1885,10 +1920,13 @@
     <t>11/09/2019</t>
   </si>
   <si>
-    <t>11/08/2019</t>
-  </si>
-  <si>
-    <t>10/09/2019</t>
+    <t>Expected Date</t>
+  </si>
+  <si>
+    <t>10/19/2017</t>
+  </si>
+  <si>
+    <t>11/20/2019</t>
   </si>
 </sst>
 </file>
@@ -1991,7 +2029,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -2007,6 +2045,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5261,9 +5300,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89930B9C-F1A9-4890-AFB9-2EA6D8CB06AA}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5961,11 +6000,41 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7BD2CEA-92A8-4DC8-8162-977D72C7275D}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE7B18D-2C9B-4C98-940D-CBDC967F6157}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6040,7 +6109,7 @@
         <v>157</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="J2" s="12" t="s">
         <v>48</v>
@@ -6059,12 +6128,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4140351F-02D4-4EFD-B194-3C3971A667AB}">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6139,7 +6208,7 @@
         <v>157</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="J2" s="12" t="s">
         <v>48</v>
@@ -6149,105 +6218,6 @@
       </c>
       <c r="L2" s="12" t="s">
         <v>170</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B8CD77E-E157-4335-960B-CEA1BA4E3EEB}">
-  <dimension ref="A1:L2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -6985,6 +6955,105 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B8CD77E-E157-4335-960B-CEA1BA4E3EEB}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045CEC76-92E4-440E-8FB5-B2D86440415F}">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -7083,7 +7152,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10EFE6F1-BD29-46DE-95C0-F9F7B6E4E4B2}">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -7182,7 +7251,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71AD8486-09F3-465F-8EC4-93F28EDF9B13}">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -7281,7 +7350,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{086590AF-81EF-4C82-958E-57A546B327AF}">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -7380,7 +7449,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B477CC7-FF3A-45A8-A37A-5798C34CD4E9}">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -7479,7 +7548,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ECCA7D5-0CE1-41A3-89D6-22D2CB3DBC2D}">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -7578,7 +7647,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F0B1588-7998-47BE-8594-1C19F016135F}">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -7677,7 +7746,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B6BA4E0-0C67-45A7-85A8-9BF5353A1E8A}">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -7776,7 +7845,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E963294-A9BA-4C6F-8828-8A0493CE8586}">
   <dimension ref="A1:L2"/>
   <sheetViews>

</xml_diff>